<commit_message>
Updated LP spec and design
</commit_message>
<xml_diff>
--- a/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.7.xlsx
+++ b/specifications/lp/Business intelligence systems - Project - Loan Portfolio Data Specification - V6.7.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ShrForms\specifications\lp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9723B0-6D17-43E9-813E-1411D73D12C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9565F11-1378-4856-AAA4-7BC40E73728F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="804" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14379,7 +14379,7 @@
   <dimension ref="A1:IQ23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15434,8 +15434,8 @@
   <dimension ref="A1:AA208"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M15" sqref="M15"/>
+      <pane ySplit="8" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>